<commit_message>
Formato HFF. Formato de KG NET/CAJA.
- Ahora se  lee la columna Sales Boxes en HFF (en lugar de Boxes).
- Ahora no hay decimales innecesarios en KG NET/CAJA en la liquidación final.
</commit_message>
<xml_diff>
--- a/data/output/program_output/liquidaciones_no_pareadas.xlsx
+++ b/data/output/program_output/liquidaciones_no_pareadas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="50">
   <si>
     <t>Observacion</t>
   </si>
@@ -100,39 +100,21 @@
     <t>No vendido</t>
   </si>
   <si>
-    <t>2024-01-29 00:00:00</t>
-  </si>
-  <si>
     <t>2023-12-22 00:00:00</t>
   </si>
   <si>
     <t>2023-12-06 00:00:00</t>
   </si>
   <si>
+    <t>2023-12-08 00:00:00</t>
+  </si>
+  <si>
     <t>1511195</t>
   </si>
   <si>
     <t>NAN</t>
   </si>
   <si>
-    <t>1513403</t>
-  </si>
-  <si>
-    <t>1513404</t>
-  </si>
-  <si>
-    <t>1513768</t>
-  </si>
-  <si>
-    <t>1513400</t>
-  </si>
-  <si>
-    <t>1513380</t>
-  </si>
-  <si>
-    <t>1513390</t>
-  </si>
-  <si>
     <t>1817</t>
   </si>
   <si>
@@ -145,30 +127,24 @@
     <t>1819</t>
   </si>
   <si>
+    <t>1861</t>
+  </si>
+  <si>
+    <t>1515904</t>
+  </si>
+  <si>
     <t>1515903</t>
   </si>
   <si>
     <t>LAPINS</t>
   </si>
   <si>
-    <t>SKEENA</t>
-  </si>
-  <si>
     <t>SANTINA</t>
   </si>
   <si>
     <t>4JD</t>
   </si>
   <si>
-    <t>XL</t>
-  </si>
-  <si>
-    <t>XLD</t>
-  </si>
-  <si>
-    <t>J-UP</t>
-  </si>
-  <si>
     <t>2J</t>
   </si>
   <si>
@@ -178,16 +154,13 @@
     <t>2JD</t>
   </si>
   <si>
+    <t>3J</t>
+  </si>
+  <si>
     <t>2JL</t>
   </si>
   <si>
     <t>2.5</t>
-  </si>
-  <si>
-    <t>5.0</t>
-  </si>
-  <si>
-    <t>10.0</t>
   </si>
   <si>
     <t>left_only</t>
@@ -548,7 +521,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V21"/>
+  <dimension ref="A1:V18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -630,16 +603,16 @@
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F2">
         <v>280</v>
       </c>
       <c r="G2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H2">
         <v>350</v>
@@ -681,7 +654,7 @@
         <v>7425.819399999999</v>
       </c>
       <c r="U2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:22">
@@ -704,7 +677,7 @@
         <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -746,36 +719,39 @@
         <v>-9.243764285714285</v>
       </c>
       <c r="U3" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:22">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
         <v>48</v>
       </c>
-      <c r="F4">
-        <v>139</v>
-      </c>
-      <c r="G4" t="s">
-        <v>56</v>
-      </c>
       <c r="H4">
-        <v>155</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>21545</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>2996.86</v>
+        <v>0</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -784,93 +760,96 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <v>859.1437317133647</v>
+        <v>12.44591904761905</v>
       </c>
       <c r="N4">
-        <v>6.180890156211257</v>
+        <v>3.111479761904762</v>
       </c>
       <c r="O4">
-        <v>1.236178031242251</v>
+        <v>1.244591904761905</v>
       </c>
       <c r="P4">
-        <v>179.8116</v>
+        <v>0</v>
       </c>
       <c r="Q4">
-        <v>1.293608633093525</v>
+        <v>0</v>
       </c>
       <c r="R4">
-        <v>0.2587217266187051</v>
+        <v>0</v>
       </c>
       <c r="S4">
-        <v>1038.955331713365</v>
+        <v>12.44591904761905</v>
       </c>
       <c r="T4">
-        <v>1957.904668286636</v>
+        <v>-12.44591904761905</v>
       </c>
       <c r="U4" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:22">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>9.260962133841391</v>
+      </c>
+      <c r="N5">
+        <v>3.08698737794713</v>
+      </c>
+      <c r="O5">
+        <v>1.234794951178852</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>9.260962133841391</v>
+      </c>
+      <c r="T5">
+        <v>-9.260962133841391</v>
+      </c>
+      <c r="U5" t="s">
         <v>49</v>
-      </c>
-      <c r="F5">
-        <v>150</v>
-      </c>
-      <c r="G5" t="s">
-        <v>56</v>
-      </c>
-      <c r="H5">
-        <v>170</v>
-      </c>
-      <c r="I5">
-        <v>25500</v>
-      </c>
-      <c r="J5">
-        <v>3546.99</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>927.1335234316886</v>
-      </c>
-      <c r="N5">
-        <v>6.180890156211257</v>
-      </c>
-      <c r="O5">
-        <v>1.236178031242251</v>
-      </c>
-      <c r="P5">
-        <v>212.8194</v>
-      </c>
-      <c r="Q5">
-        <v>1.418796</v>
-      </c>
-      <c r="R5">
-        <v>0.2837591999999999</v>
-      </c>
-      <c r="S5">
-        <v>1139.952923431689</v>
-      </c>
-      <c r="T5">
-        <v>2407.037076568311</v>
-      </c>
-      <c r="U5" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:22">
@@ -878,28 +857,28 @@
         <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F6">
-        <v>66</v>
+        <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H6">
-        <v>380</v>
+        <v>270</v>
       </c>
       <c r="I6">
-        <v>25080</v>
+        <v>270</v>
       </c>
       <c r="J6">
-        <v>3488.57</v>
+        <v>36.98630136986301</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -908,60 +887,63 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>815.877500619886</v>
+        <v>5.74247553816047</v>
       </c>
       <c r="N6">
-        <v>12.36178031242251</v>
+        <v>5.74247553816047</v>
       </c>
       <c r="O6">
-        <v>1.236178031242251</v>
+        <v>2.296990215264188</v>
       </c>
       <c r="P6">
-        <v>209.3142</v>
+        <v>2.21917808219178</v>
       </c>
       <c r="Q6">
-        <v>3.171427272727273</v>
+        <v>2.21917808219178</v>
       </c>
       <c r="R6">
-        <v>0.3171427272727273</v>
+        <v>0.8876712328767121</v>
       </c>
       <c r="S6">
-        <v>1025.191700619886</v>
+        <v>7.96165362035225</v>
       </c>
       <c r="T6">
-        <v>2463.378299380114</v>
+        <v>29.02464774951076</v>
       </c>
       <c r="U6" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:22">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
       <c r="B7" t="s">
         <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F7">
-        <v>112</v>
+        <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H7">
-        <v>370</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>41440</v>
+        <v>0</v>
       </c>
       <c r="J7">
-        <v>5764.2</v>
+        <v>0</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -970,31 +952,31 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <v>1384.519394991322</v>
+        <v>5.74247553816047</v>
       </c>
       <c r="N7">
-        <v>12.36178031242251</v>
+        <v>5.74247553816047</v>
       </c>
       <c r="O7">
-        <v>1.236178031242251</v>
+        <v>2.296990215264188</v>
       </c>
       <c r="P7">
-        <v>345.852</v>
+        <v>0</v>
       </c>
       <c r="Q7">
-        <v>3.087964285714285</v>
+        <v>0</v>
       </c>
       <c r="R7">
-        <v>0.3087964285714285</v>
+        <v>0</v>
       </c>
       <c r="S7">
-        <v>1730.371394991322</v>
+        <v>5.74247553816047</v>
       </c>
       <c r="T7">
-        <v>4033.828605008678</v>
+        <v>-5.74247553816047</v>
       </c>
       <c r="U7" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:22">
@@ -1002,28 +984,28 @@
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
         <v>45</v>
       </c>
-      <c r="E8" t="s">
-        <v>50</v>
-      </c>
       <c r="F8">
-        <v>112</v>
+        <v>279</v>
       </c>
       <c r="G8" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H8">
-        <v>360</v>
+        <v>275</v>
       </c>
       <c r="I8">
-        <v>40320</v>
+        <v>76725</v>
       </c>
       <c r="J8">
-        <v>5608.41</v>
+        <v>10510.27397260274</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -1032,31 +1014,31 @@
         <v>0</v>
       </c>
       <c r="M8">
-        <v>1384.519394991322</v>
+        <v>1602.150675146771</v>
       </c>
       <c r="N8">
-        <v>12.36178031242251</v>
+        <v>5.74247553816047</v>
       </c>
       <c r="O8">
-        <v>1.236178031242251</v>
+        <v>2.296990215264188</v>
       </c>
       <c r="P8">
-        <v>336.5046</v>
+        <v>630.6164383561644</v>
       </c>
       <c r="Q8">
-        <v>3.004505357142857</v>
+        <v>2.26027397260274</v>
       </c>
       <c r="R8">
-        <v>0.3004505357142857</v>
+        <v>0.904109589041096</v>
       </c>
       <c r="S8">
-        <v>1721.023994991322</v>
+        <v>2232.767113502935</v>
       </c>
       <c r="T8">
-        <v>3887.386005008678</v>
+        <v>8277.506859099803</v>
       </c>
       <c r="U8" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:22">
@@ -1064,158 +1046,152 @@
         <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9">
+        <v>279</v>
+      </c>
+      <c r="G9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9">
+        <v>270</v>
+      </c>
+      <c r="I9">
+        <v>75330</v>
+      </c>
+      <c r="J9">
+        <v>10319.17808219178</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>1602.150675146771</v>
+      </c>
+      <c r="N9">
+        <v>5.74247553816047</v>
+      </c>
+      <c r="O9">
+        <v>2.296990215264188</v>
+      </c>
+      <c r="P9">
+        <v>619.1506849315069</v>
+      </c>
+      <c r="Q9">
+        <v>2.219178082191781</v>
+      </c>
+      <c r="R9">
+        <v>0.8876712328767125</v>
+      </c>
+      <c r="S9">
+        <v>2221.301360078278</v>
+      </c>
+      <c r="T9">
+        <v>8097.876722113504</v>
+      </c>
+      <c r="U9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10">
+        <v>279</v>
+      </c>
+      <c r="G10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10">
+        <v>320</v>
+      </c>
+      <c r="I10">
+        <v>89280</v>
+      </c>
+      <c r="J10">
+        <v>12230.13698630137</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>1602.150675146771</v>
+      </c>
+      <c r="N10">
+        <v>5.74247553816047</v>
+      </c>
+      <c r="O10">
+        <v>2.296990215264188</v>
+      </c>
+      <c r="P10">
+        <v>733.8082191780821</v>
+      </c>
+      <c r="Q10">
+        <v>2.63013698630137</v>
+      </c>
+      <c r="R10">
+        <v>1.052054794520548</v>
+      </c>
+      <c r="S10">
+        <v>2335.958894324853</v>
+      </c>
+      <c r="T10">
+        <v>9894.178091976517</v>
+      </c>
+      <c r="U10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" t="s">
         <v>45</v>
       </c>
-      <c r="E9" t="s">
-        <v>50</v>
-      </c>
-      <c r="F9">
-        <v>112</v>
-      </c>
-      <c r="G9" t="s">
-        <v>57</v>
-      </c>
-      <c r="H9">
-        <v>360</v>
-      </c>
-      <c r="I9">
-        <v>40320</v>
-      </c>
-      <c r="J9">
-        <v>5608.41</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>1384.519394991322</v>
-      </c>
-      <c r="N9">
-        <v>12.36178031242251</v>
-      </c>
-      <c r="O9">
-        <v>1.236178031242251</v>
-      </c>
-      <c r="P9">
-        <v>336.5046</v>
-      </c>
-      <c r="Q9">
-        <v>3.004505357142857</v>
-      </c>
-      <c r="R9">
-        <v>0.3004505357142857</v>
-      </c>
-      <c r="S9">
-        <v>1721.023994991322</v>
-      </c>
-      <c r="T9">
-        <v>3887.386005008678</v>
-      </c>
-      <c r="U9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22">
-      <c r="A10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10">
-        <v>4</v>
-      </c>
-      <c r="G10" t="s">
-        <v>55</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>12.44591904761905</v>
-      </c>
-      <c r="N10">
-        <v>3.111479761904762</v>
-      </c>
-      <c r="O10">
-        <v>1.244591904761905</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="R10">
-        <v>0</v>
-      </c>
-      <c r="S10">
-        <v>12.44591904761905</v>
-      </c>
-      <c r="T10">
-        <v>-12.44591904761905</v>
-      </c>
-      <c r="U10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" t="s">
-        <v>32</v>
-      </c>
       <c r="F11">
-        <v>3</v>
+        <v>280</v>
       </c>
       <c r="G11" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>275</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>77000</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>10547.94520547945</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -1224,60 +1200,60 @@
         <v>0</v>
       </c>
       <c r="M11">
-        <v>9.260962133841391</v>
+        <v>1607.893150684931</v>
       </c>
       <c r="N11">
-        <v>3.08698737794713</v>
+        <v>5.74247553816047</v>
       </c>
       <c r="O11">
-        <v>1.234794951178852</v>
+        <v>2.296990215264188</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <v>632.8767123287671</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>2.260273972602739</v>
       </c>
       <c r="R11">
-        <v>0</v>
+        <v>0.9041095890410957</v>
       </c>
       <c r="S11">
-        <v>9.260962133841391</v>
+        <v>2240.769863013698</v>
       </c>
       <c r="T11">
-        <v>-9.260962133841391</v>
+        <v>8307.175342465755</v>
       </c>
       <c r="U11" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:22">
       <c r="B12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F12">
         <v>280</v>
       </c>
       <c r="G12" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H12">
-        <v>270</v>
+        <v>300</v>
       </c>
       <c r="I12">
-        <v>270</v>
+        <v>84000</v>
       </c>
       <c r="J12">
-        <v>36.98630136986301</v>
+        <v>11506.84931506849</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -1286,31 +1262,31 @@
         <v>0</v>
       </c>
       <c r="M12">
-        <v>1148.495107632094</v>
+        <v>1607.893150684931</v>
       </c>
       <c r="N12">
-        <v>4.101768241543192</v>
+        <v>5.74247553816047</v>
       </c>
       <c r="O12">
-        <v>1.640707296617277</v>
+        <v>2.296990215264188</v>
       </c>
       <c r="P12">
-        <v>2.21917808219178</v>
+        <v>690.4109589041096</v>
       </c>
       <c r="Q12">
-        <v>0.007925636007827787</v>
+        <v>2.465753424657534</v>
       </c>
       <c r="R12">
-        <v>0.003170254403131115</v>
+        <v>0.9863013698630138</v>
       </c>
       <c r="S12">
-        <v>1150.714285714286</v>
+        <v>2298.304109589041</v>
       </c>
       <c r="T12">
-        <v>-1113.727984344423</v>
+        <v>9208.545205479451</v>
       </c>
       <c r="U12" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:22">
@@ -1318,22 +1294,22 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
         <v>40</v>
       </c>
-      <c r="D13" t="s">
-        <v>44</v>
-      </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F13">
-        <v>280</v>
+        <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -1351,13 +1327,13 @@
         <v>0</v>
       </c>
       <c r="M13">
-        <v>1148.495107632094</v>
+        <v>5.74247553816047</v>
       </c>
       <c r="N13">
-        <v>4.101768241543192</v>
+        <v>5.74247553816047</v>
       </c>
       <c r="O13">
-        <v>1.640707296617277</v>
+        <v>2.296990215264188</v>
       </c>
       <c r="P13">
         <v>0</v>
@@ -1369,42 +1345,45 @@
         <v>0</v>
       </c>
       <c r="S13">
-        <v>1148.495107632094</v>
+        <v>5.74247553816047</v>
       </c>
       <c r="T13">
-        <v>-1148.495107632094</v>
+        <v>-5.74247553816047</v>
       </c>
       <c r="U13" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:22">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
       <c r="B14" t="s">
         <v>29</v>
       </c>
       <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
         <v>41</v>
       </c>
-      <c r="D14" t="s">
-        <v>44</v>
-      </c>
       <c r="E14" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F14">
-        <v>280</v>
+        <v>15</v>
       </c>
       <c r="G14" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H14">
-        <v>275</v>
+        <v>330</v>
       </c>
       <c r="I14">
-        <v>76725</v>
+        <v>4950</v>
       </c>
       <c r="J14">
-        <v>10510.27397260274</v>
+        <v>678.082191780822</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -1413,34 +1392,37 @@
         <v>0</v>
       </c>
       <c r="M14">
-        <v>1148.495107632094</v>
+        <v>68.69757827788649</v>
       </c>
       <c r="N14">
-        <v>4.101768241543192</v>
+        <v>4.579838551859099</v>
       </c>
       <c r="O14">
-        <v>1.640707296617277</v>
+        <v>1.83193542074364</v>
       </c>
       <c r="P14">
-        <v>630.6164383561644</v>
+        <v>40.68493150684932</v>
       </c>
       <c r="Q14">
-        <v>2.25220156555773</v>
+        <v>2.712328767123288</v>
       </c>
       <c r="R14">
-        <v>0.900880626223092</v>
+        <v>1.084931506849315</v>
       </c>
       <c r="S14">
-        <v>1779.111545988258</v>
+        <v>109.3825097847358</v>
       </c>
       <c r="T14">
-        <v>8731.162426614481</v>
+        <v>568.6996819960862</v>
       </c>
       <c r="U14" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:22">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
       <c r="B15" t="s">
         <v>29</v>
       </c>
@@ -1448,25 +1430,25 @@
         <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F15">
-        <v>280</v>
+        <v>256</v>
       </c>
       <c r="G15" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H15">
-        <v>270</v>
+        <v>340</v>
       </c>
       <c r="I15">
-        <v>75330</v>
+        <v>87040</v>
       </c>
       <c r="J15">
-        <v>10319.17808219178</v>
+        <v>11923.28767123288</v>
       </c>
       <c r="K15">
         <v>0</v>
@@ -1475,60 +1457,63 @@
         <v>0</v>
       </c>
       <c r="M15">
-        <v>1148.495107632094</v>
+        <v>1172.438669275929</v>
       </c>
       <c r="N15">
-        <v>4.101768241543192</v>
+        <v>4.579838551859099</v>
       </c>
       <c r="O15">
-        <v>1.640707296617277</v>
+        <v>1.83193542074364</v>
       </c>
       <c r="P15">
-        <v>619.1506849315069</v>
+        <v>715.3972602739725</v>
       </c>
       <c r="Q15">
-        <v>2.211252446183953</v>
+        <v>2.794520547945205</v>
       </c>
       <c r="R15">
-        <v>0.8845009784735813</v>
+        <v>1.117808219178082</v>
       </c>
       <c r="S15">
-        <v>1767.645792563601</v>
+        <v>1887.835929549902</v>
       </c>
       <c r="T15">
-        <v>8551.532289628181</v>
+        <v>10035.45174168297</v>
       </c>
       <c r="U15" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:22">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
       <c r="B16" t="s">
         <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F16">
-        <v>280</v>
+        <v>4</v>
       </c>
       <c r="G16" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H16">
-        <v>320</v>
+        <v>350</v>
       </c>
       <c r="I16">
-        <v>89280</v>
+        <v>1400</v>
       </c>
       <c r="J16">
-        <v>12230.13698630137</v>
+        <v>191.7808219178083</v>
       </c>
       <c r="K16">
         <v>0</v>
@@ -1537,60 +1522,63 @@
         <v>0</v>
       </c>
       <c r="M16">
-        <v>1148.495107632094</v>
+        <v>18.3193542074364</v>
       </c>
       <c r="N16">
-        <v>4.101768241543192</v>
+        <v>4.579838551859099</v>
       </c>
       <c r="O16">
-        <v>1.640707296617277</v>
+        <v>1.83193542074364</v>
       </c>
       <c r="P16">
-        <v>733.8082191780821</v>
+        <v>11.50684931506849</v>
       </c>
       <c r="Q16">
-        <v>2.620743639921722</v>
+        <v>2.876712328767124</v>
       </c>
       <c r="R16">
-        <v>1.048297455968689</v>
+        <v>1.150684931506849</v>
       </c>
       <c r="S16">
-        <v>1882.303326810176</v>
+        <v>29.82620352250489</v>
       </c>
       <c r="T16">
-        <v>10347.83365949119</v>
+        <v>161.9546183953034</v>
       </c>
       <c r="U16" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:21">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
       <c r="B17" t="s">
         <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E17" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F17">
-        <v>280</v>
+        <v>20</v>
       </c>
       <c r="G17" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H17">
-        <v>275</v>
+        <v>350</v>
       </c>
       <c r="I17">
-        <v>77000</v>
+        <v>7000</v>
       </c>
       <c r="J17">
-        <v>10547.94520547945</v>
+        <v>958.9041095890412</v>
       </c>
       <c r="K17">
         <v>0</v>
@@ -1599,63 +1587,63 @@
         <v>0</v>
       </c>
       <c r="M17">
-        <v>1148.495107632094</v>
+        <v>91.59677103718198</v>
       </c>
       <c r="N17">
-        <v>4.101768241543192</v>
+        <v>4.579838551859099</v>
       </c>
       <c r="O17">
-        <v>1.640707296617277</v>
+        <v>1.83193542074364</v>
       </c>
       <c r="P17">
-        <v>632.8767123287671</v>
+        <v>57.53424657534247</v>
       </c>
       <c r="Q17">
-        <v>2.260273972602739</v>
+        <v>2.876712328767124</v>
       </c>
       <c r="R17">
-        <v>0.9041095890410957</v>
+        <v>1.150684931506849</v>
       </c>
       <c r="S17">
-        <v>1781.371819960861</v>
+        <v>149.1310176125245</v>
       </c>
       <c r="T17">
-        <v>8766.573385518592</v>
+        <v>809.7730919765168</v>
       </c>
       <c r="U17" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:21">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" t="s">
         <v>41</v>
       </c>
-      <c r="D18" t="s">
-        <v>44</v>
-      </c>
       <c r="E18" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F18">
-        <v>280</v>
+        <v>15</v>
       </c>
       <c r="G18" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>315</v>
       </c>
       <c r="I18">
-        <v>0</v>
+        <v>4725</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>647.2602739726027</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -1664,226 +1652,31 @@
         <v>0</v>
       </c>
       <c r="M18">
-        <v>1148.495107632094</v>
+        <v>68.69757827788649</v>
       </c>
       <c r="N18">
-        <v>4.101768241543192</v>
+        <v>4.579838551859099</v>
       </c>
       <c r="O18">
-        <v>1.640707296617277</v>
+        <v>1.83193542074364</v>
       </c>
       <c r="P18">
-        <v>0</v>
+        <v>38.83561643835616</v>
       </c>
       <c r="Q18">
-        <v>0</v>
+        <v>2.589041095890411</v>
       </c>
       <c r="R18">
-        <v>0</v>
+        <v>1.035616438356164</v>
       </c>
       <c r="S18">
-        <v>1148.495107632094</v>
+        <v>107.5331947162427</v>
       </c>
       <c r="T18">
-        <v>-1148.495107632094</v>
+        <v>539.7270792563601</v>
       </c>
       <c r="U18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21">
-      <c r="A19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" t="s">
-        <v>54</v>
-      </c>
-      <c r="F19">
-        <v>280</v>
-      </c>
-      <c r="G19" t="s">
-        <v>55</v>
-      </c>
-      <c r="H19">
-        <v>340</v>
-      </c>
-      <c r="I19">
-        <v>87040</v>
-      </c>
-      <c r="J19">
-        <v>11923.28767123288</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19">
-        <v>915.9677103718199</v>
-      </c>
-      <c r="N19">
-        <v>3.271313251327928</v>
-      </c>
-      <c r="O19">
-        <v>1.308525300531171</v>
-      </c>
-      <c r="P19">
-        <v>715.3972602739725</v>
-      </c>
-      <c r="Q19">
-        <v>2.554990215264187</v>
-      </c>
-      <c r="R19">
-        <v>1.021996086105675</v>
-      </c>
-      <c r="S19">
-        <v>1631.364970645792</v>
-      </c>
-      <c r="T19">
-        <v>10291.92270058708</v>
-      </c>
-      <c r="U19" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21">
-      <c r="A20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" t="s">
-        <v>54</v>
-      </c>
-      <c r="F20">
-        <v>280</v>
-      </c>
-      <c r="G20" t="s">
-        <v>55</v>
-      </c>
-      <c r="H20">
-        <v>350</v>
-      </c>
-      <c r="I20">
-        <v>1400</v>
-      </c>
-      <c r="J20">
-        <v>191.7808219178083</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20">
-        <v>915.9677103718199</v>
-      </c>
-      <c r="N20">
-        <v>3.271313251327928</v>
-      </c>
-      <c r="O20">
-        <v>1.308525300531171</v>
-      </c>
-      <c r="P20">
-        <v>11.50684931506849</v>
-      </c>
-      <c r="Q20">
-        <v>0.04109589041095891</v>
-      </c>
-      <c r="R20">
-        <v>0.01643835616438356</v>
-      </c>
-      <c r="S20">
-        <v>927.4745596868884</v>
-      </c>
-      <c r="T20">
-        <v>-735.6937377690801</v>
-      </c>
-      <c r="U20" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21">
-      <c r="A21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" t="s">
-        <v>54</v>
-      </c>
-      <c r="F21">
-        <v>280</v>
-      </c>
-      <c r="G21" t="s">
-        <v>55</v>
-      </c>
-      <c r="H21">
-        <v>350</v>
-      </c>
-      <c r="I21">
-        <v>7000</v>
-      </c>
-      <c r="J21">
-        <v>958.9041095890412</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21">
-        <v>915.9677103718199</v>
-      </c>
-      <c r="N21">
-        <v>3.271313251327928</v>
-      </c>
-      <c r="O21">
-        <v>1.308525300531171</v>
-      </c>
-      <c r="P21">
-        <v>57.53424657534247</v>
-      </c>
-      <c r="Q21">
-        <v>0.2054794520547945</v>
-      </c>
-      <c r="R21">
-        <v>0.08219178082191782</v>
-      </c>
-      <c r="S21">
-        <v>973.5019569471623</v>
-      </c>
-      <c r="T21">
-        <v>-14.59784735812104</v>
-      </c>
-      <c r="U21" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>